<commit_message>
Updated Browser, Shop (added check gost on site), updated Text (check gost)
</commit_message>
<xml_diff>
--- a/source/poiskpostav_v1_test.xlsx
+++ b/source/poiskpostav_v1_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142867D9-F571-45BE-9FBA-02A24AE3D065}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B885751D-A526-4F58-B4DB-102780B32D60}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>* Манжета М220х250 ГОСТ 22704</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>* БОЛТ; СТАНДАРТ ГОСТ Р ИСО4014 DIN931 (ГОСТ7798/7805), ГОЛОВКА ШЕСТИГРАННАЯ, ОБОЗНАЧЕНИЕ M16Х65, КЛАСС ПРОЧНОСТИ 8.8, МАТЕРИАЛ СТАЛЬ ОЦИНКОВАННАЯ</t>
+  </si>
+  <si>
+    <t>* Гайка шестигранная M20х1,5.5 покрытие цинковое, хроматированное ГОСТ 15521</t>
   </si>
 </sst>
 </file>
@@ -364,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,54 +389,62 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8"/>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
folder "html_for_tests" renamed to "files_for_tests" and added files "market_links_(1-3)", added file main_test.py for tests, changed xlsx file "poiskpostav_v1_test.xlsx"
</commit_message>
<xml_diff>
--- a/source/poiskpostav_v1_test.xlsx
+++ b/source/poiskpostav_v1_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B885751D-A526-4F58-B4DB-102780B32D60}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E168206-4203-4913-AA25-ADC5F5731778}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,22 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>* Манжета М220х250 ГОСТ 22704</t>
-  </si>
-  <si>
-    <t>* Рукав с текстильным каркасом ВГ(III)-10-25-38-У ГОСТ 18698</t>
-  </si>
-  <si>
-    <t>* БОЛТ; СТАНДАРТ ГОСТ7796, ГОЛОВКА ШЕСТИГРАННАЯ, ОБОЗНАЧЕНИЕ M20Х80, КЛАСС ПРОЧНОСТИ 6.6, МАТЕРИАЛ СТАЛЬ ОЦИНКОВАННАЯ</t>
-  </si>
-  <si>
-    <t>* Гайка шестигранная M30.8.35 покрытие цинковое ГОСТ 15521</t>
-  </si>
-  <si>
-    <t>* ШАЙБА; ТИП ПЛОСКАЯ УМЕНЬШЕННАЯ, СТАНДАРТ ГОСТ10450 DIN433, ОБОЗНАЧЕНИЕ А24, МАТЕРИАЛ СТАЛЬ 20 ОЦИНКОВАННАЯ</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Наименование</t>
   </si>
@@ -43,10 +28,13 @@
     <t>№</t>
   </si>
   <si>
-    <t>* БОЛТ; СТАНДАРТ ГОСТ Р ИСО4014 DIN931 (ГОСТ7798/7805), ГОЛОВКА ШЕСТИГРАННАЯ, ОБОЗНАЧЕНИЕ M16Х65, КЛАСС ПРОЧНОСТИ 8.8, МАТЕРИАЛ СТАЛЬ ОЦИНКОВАННАЯ</t>
+    <t>* Манжета М60х80 ГОСТ 22704</t>
   </si>
   <si>
-    <t>* Гайка шестигранная M20х1,5.5 покрытие цинковое, хроматированное ГОСТ 15521</t>
+    <t>* Рукав газосварочный I-6,3-0,63-У ГОСТ 9356</t>
+  </si>
+  <si>
+    <t>* Гвоздь строительный круглый головка плоская 3х80 ГОСТ 4028</t>
   </si>
 </sst>
 </file>
@@ -370,7 +358,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,67 +369,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
+      <c r="B5"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
+      <c r="B6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
+      <c r="B7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
+      <c r="B8"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9"/>

</xml_diff>

<commit_message>
Fix excel text file
True line number
</commit_message>
<xml_diff>
--- a/source/poiskpostav_v1_test.xlsx
+++ b/source/poiskpostav_v1_test.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E168206-4203-4913-AA25-ADC5F5731778}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\npara\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B471FD2A-7E70-4C10-A3FC-AC32DEE42154}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11805" xr2:uid="{B8758886-7B89-4A0C-B589-C8802E01DCE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,10 +27,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Наименование</t>
+    <t>№</t>
   </si>
   <si>
-    <t>№</t>
+    <t>Наименование</t>
   </si>
   <si>
     <t>* Манжета М60х80 ГОСТ 22704</t>
@@ -47,6 +52,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -70,11 +76,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -109,7 +112,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -121,7 +124,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -168,6 +171,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -203,6 +223,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -354,25 +391,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5203C9-2AE8-41F4-BC49-59731A22175E}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="77.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -399,23 +432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commented and code cleaned class_Excel.py and class_Browser.py
</commit_message>
<xml_diff>
--- a/source/poiskpostav_v1_test.xlsx
+++ b/source/poiskpostav_v1_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E168206-4203-4913-AA25-ADC5F5731778}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91658B21-AEFF-494F-90A2-946EBF26577A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3720" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -355,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A5" sqref="A5:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,21 +399,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>